<commit_message>
Time Based Extration part completed
</commit_message>
<xml_diff>
--- a/R-Date and Time Functions/R_DateandTimeFunctions.xlsx
+++ b/R-Date and Time Functions/R_DateandTimeFunctions.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulus\Desktop\Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulus\Documents\GitHub\R-Codes\R-Date and Time Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A720BA-5D4B-49DA-9A7D-70E80D6BD864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5A98F-BD2F-4D25-AB94-DE798760DD39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{F01CDF7E-9884-4A70-B21E-814D077F94A5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="General" sheetId="2" r:id="rId1"/>
+    <sheet name="Extractions" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Extractions!$B$2:$C$14</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">Sys.Date()                        </t>
   </si>
@@ -41,9 +42,6 @@
     <t>Sys.time()</t>
   </si>
   <si>
-    <t>Show current Date &amp; timestamp</t>
-  </si>
-  <si>
     <t>format(Sys.time(),format = '%T')</t>
   </si>
   <si>
@@ -53,9 +51,6 @@
     <t>as.Date(Sys.time())</t>
   </si>
   <si>
-    <t xml:space="preserve">Casting  timestamp as date </t>
-  </si>
-  <si>
     <t xml:space="preserve">format(Sys.time(),format= '%d')  </t>
   </si>
   <si>
@@ -92,12 +87,6 @@
     <t>Extracting Weeknumber from timestamp</t>
   </si>
   <si>
-    <t>format(Sys.time(),format= '%U')</t>
-  </si>
-  <si>
-    <t>Extracting ISO Weeknumber from timestamp</t>
-  </si>
-  <si>
     <t>weekdays(Sys.time())</t>
   </si>
   <si>
@@ -111,6 +100,120 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::day(Sys.time())             </t>
+  </si>
+  <si>
+    <t>lubridate::month(Sys.Date())</t>
+  </si>
+  <si>
+    <t>lubridate::quarter(Sys.time())</t>
+  </si>
+  <si>
+    <t>lubridate::year(Sys.time())</t>
+  </si>
+  <si>
+    <t>lubridate::week(Sys.Date())</t>
+  </si>
+  <si>
+    <t>Show timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casting timestamp as date </t>
+  </si>
+  <si>
+    <t>Extracting day of the year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::yday(Sys.Date()) </t>
+  </si>
+  <si>
+    <t>Extracting day of the month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::mday(Sys.Date())       </t>
+  </si>
+  <si>
+    <t>Extracting day of the quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::qday(Sys.Date())       </t>
+  </si>
+  <si>
+    <t>Gets fiscal quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::quarter(Sys.Date())    </t>
+  </si>
+  <si>
+    <t>Extracting day of the week(Start start day: Sunday)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::wday(Sys.Date())       </t>
+  </si>
+  <si>
+    <t>Validates if a time is AM or PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::am(Sys.time())         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::leap_year(2020)        </t>
+  </si>
+  <si>
+    <t>Validates for leap year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::floor_date(Sys.Date(),unit = "week")    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::floor_date(Sys.Date(),unit = "month")   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::floor_date(Sys.Date(),unit = "year")    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::ceiling_date(Sys.Date(),unit = 'week')  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::ceiling_date(Sys.Date(),unit = 'month') </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubridate::ceiling_date(Sys.Date(),unit = 'year')  </t>
+  </si>
+  <si>
+    <t>Week start date</t>
+  </si>
+  <si>
+    <t>Month start date</t>
+  </si>
+  <si>
+    <t>Year start date</t>
+  </si>
+  <si>
+    <t>Week end date</t>
+  </si>
+  <si>
+    <t>Month end date</t>
+  </si>
+  <si>
+    <t>Year end date</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Packages Used</t>
+  </si>
+  <si>
+    <t>Base,Lubridate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional useful packages </t>
+  </si>
+  <si>
+    <t>chron</t>
   </si>
 </sst>
 </file>
@@ -154,9 +257,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -471,125 +573,353 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66377FBE-46D8-40CD-8275-9ACB60AF0175}">
-  <dimension ref="B2:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B66637-788A-4423-9DDD-91E52CA5D229}">
+  <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66377FBE-46D8-40CD-8275-9ACB60AF0175}">
+  <dimension ref="A2:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:C14" xr:uid="{E4202F93-1BDA-45FA-B300-AEF778082AFC}"/>

</xml_diff>

<commit_message>
Updated the missed extraction part and added Time Formats
Need to add date formats
</commit_message>
<xml_diff>
--- a/R-Date and Time Functions/R_DateandTimeFunctions.xlsx
+++ b/R-Date and Time Functions/R_DateandTimeFunctions.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulus\Documents\GitHub\R-Codes\R-Date and Time Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE819320-A55E-475C-B5D1-FD78250034F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F21EC62-6C82-451E-817D-0F28074B6055}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{F01CDF7E-9884-4A70-B21E-814D077F94A5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{F01CDF7E-9884-4A70-B21E-814D077F94A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
     <sheet name="Extractions" sheetId="1" r:id="rId2"/>
+    <sheet name="Time &amp; Date Formats " sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Extractions!$B$2:$C$14</definedName>
@@ -594,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B66637-788A-4423-9DDD-91E52CA5D229}">
   <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66377FBE-46D8-40CD-8275-9ACB60AF0175}">
   <dimension ref="A2:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,4 +978,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676F66C7-F48B-478F-983B-1B014FC7CA70}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>